<commit_message>
birat 2010-based steel scenarios and factories upstream fuel units CCS units squashed bugs in flow naming
</commit_message>
<xml_diff>
--- a/data/shared/CCS_calc.xlsx
+++ b/data/shared/CCS_calc.xlsx
@@ -15,6 +15,7 @@
     <sheet name="CO2 Capture" sheetId="2" r:id="rId1"/>
     <sheet name="CO2 Compression" sheetId="5" r:id="rId2"/>
     <sheet name="CO2 Cap-Compress" sheetId="4" r:id="rId3"/>
+    <sheet name="bb CO2 storage" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="36">
   <si>
     <t>Heat Demand</t>
   </si>
@@ -55,12 +56,6 @@
     <t>Outflows</t>
   </si>
   <si>
-    <t>Captured CO2</t>
-  </si>
-  <si>
-    <t>CO2__Compressed</t>
-  </si>
-  <si>
     <t>CO2 Compression Efficiency</t>
   </si>
   <si>
@@ -91,12 +86,6 @@
     <t>meta-notes</t>
   </si>
   <si>
-    <t>captured CO2</t>
-  </si>
-  <si>
-    <t>compressed CO2</t>
-  </si>
-  <si>
     <t>electricity</t>
   </si>
   <si>
@@ -116,15 +105,66 @@
   </si>
   <si>
     <t>CONSUMED__electricity</t>
+  </si>
+  <si>
+    <t>CO2__collected</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>% CO2 Collected</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Ancillary Emissions</t>
+  </si>
+  <si>
+    <t>CO2__compressed</t>
+  </si>
+  <si>
+    <t>carbon and oxygen</t>
+  </si>
+  <si>
+    <t>CO2__stored</t>
+  </si>
+  <si>
+    <t>CO2__emitted</t>
+  </si>
+  <si>
+    <t>CO2__captured</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -166,6 +206,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,15 +233,21 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -512,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,143 +584,197 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="D6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="F7" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -676,7 +783,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -688,42 +795,42 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
+      <c r="A2" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
+      <c r="C2" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -732,18 +839,18 @@
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>21</v>
+      <c r="A3" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
+      <c r="C3" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -752,18 +859,18 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
+      <c r="A4" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -776,14 +883,14 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>22</v>
+      <c r="A5" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -797,36 +904,36 @@
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -836,10 +943,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,145 +962,318 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="F2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>